<commit_message>
Final changes with integrated app
</commit_message>
<xml_diff>
--- a/chatbot_train.xlsx
+++ b/chatbot_train.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>

</xml_diff>